<commit_message>
Implemetation of wait in progress
</commit_message>
<xml_diff>
--- a/src/test/java/com/clearMechanic/data/ClearMechanic.xlsx
+++ b/src/test/java/com/clearMechanic/data/ClearMechanic.xlsx
@@ -14,9 +14,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>VIN Number</t>
+  </si>
+  <si>
+    <t>8LDC2230CE021610</t>
+  </si>
+  <si>
+    <t>8LDC2230CE021641</t>
+  </si>
+  <si>
+    <t>KNAPM81ABG7000347</t>
+  </si>
+  <si>
+    <t>KNALN414BB5015438</t>
+  </si>
+  <si>
+    <t>KNALN414BC5079465</t>
+  </si>
+  <si>
+    <t>KNAHU812AH7158037</t>
+  </si>
+  <si>
+    <t>KNAFT411BD5785277</t>
+  </si>
+  <si>
+    <t>KNAMC812BG6082657</t>
+  </si>
+  <si>
+    <t>KNALD225385130724</t>
+  </si>
+  <si>
+    <t>KNABX512BCT035612</t>
+  </si>
+  <si>
+    <t>KNALT412BE6010919</t>
+  </si>
+  <si>
+    <t>KNAMB761286195778</t>
+  </si>
+  <si>
+    <t>KNAJX81EFF7000871</t>
+  </si>
+  <si>
+    <t>8LCDC22328E008536</t>
   </si>
 </sst>
 </file>
@@ -381,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -392,36 +434,79 @@
     <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>4564</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>3423</v>
-      </c>
-      <c r="B2">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>4354</v>
-      </c>
-      <c r="B3">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>54654</v>
-      </c>
-      <c r="B4">
-        <v>46456</v>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>